<commit_message>
CIERRE 16 DIC 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #10 OCTUBRE 2023/INVENTARIO ALMACEN  OCTUBRE  -2023 rtr.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #10 OCTUBRE 2023/INVENTARIO ALMACEN  OCTUBRE  -2023 rtr.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20925" windowHeight="11745" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20925" windowHeight="11745" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name=" E N E R O    2 0 2 3      " sheetId="1" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <sheet name="  A G O S TO      2 0 2 3      " sheetId="9" r:id="rId8"/>
     <sheet name="SEPTIEMBRE     2 0 2 3        " sheetId="10" r:id="rId9"/>
     <sheet name="  OCTUBRE    2 0 2 3        " sheetId="11" r:id="rId10"/>
-    <sheet name="Hoja4" sheetId="12" r:id="rId11"/>
+    <sheet name="  NOVIEMBRE   2 0 2 3          " sheetId="12" r:id="rId11"/>
+    <sheet name="Hoja1" sheetId="13" r:id="rId12"/>
+    <sheet name="Hoja2" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -340,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="166">
   <si>
     <t>INVENTARIO ALMACEN</t>
   </si>
@@ -887,6 +889,36 @@
   <si>
     <t>Bety DIF X MAL REGISTRO EN 270 E1 DE      0.40 kg</t>
   </si>
+  <si>
+    <t>Oct-,2023</t>
+  </si>
+  <si>
+    <t>Nov-,2023</t>
+  </si>
+  <si>
+    <t>CONTRA FRIBOY</t>
+  </si>
+  <si>
+    <t>COSTILLA ESPECIAL  DE CERDO</t>
+  </si>
+  <si>
+    <t>ESPALDILLA  C/H</t>
+  </si>
+  <si>
+    <t>T-BONE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAVOS NATURAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR DE BETY EN REGISTO NOTA  420  deben ser 5 CAJAS </t>
+  </si>
+  <si>
+    <t>BETY NO DIO DE BAJA EL TRASPASO  541 E1</t>
+  </si>
+  <si>
+    <t>ERROR DE BETY REGISTRO 1 CAJA MENOS</t>
+  </si>
 </sst>
 </file>
 
@@ -1323,7 +1355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1480,6 +1512,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="125">
     <border>
@@ -3077,7 +3115,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="727">
+  <cellXfs count="744">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4749,6 +4787,75 @@
     <xf numFmtId="0" fontId="11" fillId="14" borderId="124" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="124" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4785,48 +4892,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4926,6 +4991,21 @@
     <xf numFmtId="1" fontId="30" fillId="0" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="30" fillId="8" borderId="114" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="30" fillId="8" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="30" fillId="8" borderId="114" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="30" fillId="8" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="124" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4944,21 +5024,6 @@
     <xf numFmtId="0" fontId="12" fillId="26" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="30" fillId="8" borderId="114" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="30" fillId="8" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="30" fillId="8" borderId="114" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="30" fillId="8" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="124" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="42" fillId="0" borderId="114" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4970,6 +5035,30 @@
     </xf>
     <xf numFmtId="1" fontId="42" fillId="0" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="8" borderId="61" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="8" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="124" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="124" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4981,6 +5070,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99CCFF"/>
+      <color rgb="FF800000"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FF66FF99"/>
       <color rgb="FF66FF66"/>
@@ -4988,9 +5079,7 @@
       <color rgb="FFCCCCFF"/>
       <color rgb="FF00CC00"/>
       <color rgb="FF00FFCC"/>
-      <color rgb="FF800000"/>
       <color rgb="FFCC99FF"/>
-      <color rgb="FF9999FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -5407,10 +5496,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="653" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="654"/>
+      <c r="B1" s="676" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="677"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -5422,21 +5511,21 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="655">
+      <c r="B2" s="678">
         <v>44955</v>
       </c>
-      <c r="C2" s="656"/>
-      <c r="F2" s="657" t="s">
+      <c r="C2" s="679"/>
+      <c r="F2" s="680" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="657"/>
-      <c r="H2" s="657"/>
+      <c r="G2" s="680"/>
+      <c r="H2" s="680"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
-      <c r="K2" s="658" t="s">
+      <c r="K2" s="681" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="658"/>
+      <c r="L2" s="681"/>
       <c r="M2" s="9"/>
       <c r="N2" s="10"/>
       <c r="Q2" s="12"/>
@@ -5446,30 +5535,30 @@
     </row>
     <row r="3" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="659" t="s">
+      <c r="C3" s="682" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="660"/>
+      <c r="D3" s="683"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="661" t="s">
+      <c r="F3" s="684" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="662"/>
+      <c r="G3" s="685"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="663" t="s">
+      <c r="I3" s="686" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="16"/>
-      <c r="K3" s="658"/>
-      <c r="L3" s="658"/>
-      <c r="M3" s="666" t="s">
+      <c r="K3" s="681"/>
+      <c r="L3" s="681"/>
+      <c r="M3" s="663" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="667"/>
-      <c r="O3" s="668" t="s">
+      <c r="N3" s="664"/>
+      <c r="O3" s="665" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="669"/>
+      <c r="P3" s="666"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
@@ -5495,7 +5584,7 @@
       <c r="H4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="664"/>
+      <c r="I4" s="687"/>
       <c r="J4" s="16"/>
       <c r="K4" s="21" t="s">
         <v>10</v>
@@ -5556,8 +5645,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="670"/>
-      <c r="P5" s="670"/>
+      <c r="O5" s="667"/>
+      <c r="P5" s="667"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
@@ -5599,8 +5688,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O6" s="671"/>
-      <c r="P6" s="671"/>
+      <c r="O6" s="668"/>
+      <c r="P6" s="668"/>
       <c r="Q6" s="45"/>
       <c r="R6" s="13"/>
       <c r="S6" s="46"/>
@@ -5683,8 +5772,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O8" s="672"/>
-      <c r="P8" s="672"/>
+      <c r="O8" s="669"/>
+      <c r="P8" s="669"/>
       <c r="Q8" s="45"/>
       <c r="R8" s="13"/>
       <c r="S8" s="13"/>
@@ -5765,8 +5854,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O10" s="673"/>
-      <c r="P10" s="673"/>
+      <c r="O10" s="670"/>
+      <c r="P10" s="670"/>
       <c r="Q10" s="45"/>
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
@@ -5894,8 +5983,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O13" s="674"/>
-      <c r="P13" s="674"/>
+      <c r="O13" s="671"/>
+      <c r="P13" s="671"/>
       <c r="Q13" s="45"/>
       <c r="R13" s="66"/>
       <c r="S13" s="66"/>
@@ -6163,8 +6252,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O20" s="675"/>
-      <c r="P20" s="675"/>
+      <c r="O20" s="672"/>
+      <c r="P20" s="672"/>
       <c r="Q20" s="45"/>
       <c r="R20" s="13"/>
       <c r="S20" s="13"/>
@@ -6249,8 +6338,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O22" s="676"/>
-      <c r="P22" s="676"/>
+      <c r="O22" s="673"/>
+      <c r="P22" s="673"/>
       <c r="Q22" s="45"/>
       <c r="R22" s="78"/>
       <c r="S22" s="78"/>
@@ -6292,8 +6381,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O23" s="677"/>
-      <c r="P23" s="677"/>
+      <c r="O23" s="674"/>
+      <c r="P23" s="674"/>
       <c r="Q23" s="45"/>
       <c r="R23" s="13"/>
       <c r="S23" s="13"/>
@@ -6415,8 +6504,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O26" s="678"/>
-      <c r="P26" s="678"/>
+      <c r="O26" s="675"/>
+      <c r="P26" s="675"/>
       <c r="Q26" s="45"/>
       <c r="R26" s="13"/>
       <c r="S26" s="13"/>
@@ -6929,10 +7018,10 @@
     <row r="40" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="145"/>
       <c r="D40" s="147"/>
-      <c r="F40" s="665" t="s">
+      <c r="F40" s="662" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="665"/>
+      <c r="G40" s="662"/>
       <c r="H40" s="148">
         <f>SUM(H5:H31)</f>
         <v>51250.14</v>
@@ -7132,6 +7221,13 @@
     <sortCondition ref="B5:B38"/>
   </sortState>
   <mergeCells count="19">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
@@ -7144,13 +7240,6 @@
     <mergeCell ref="O22:P22"/>
     <mergeCell ref="O23:P23"/>
     <mergeCell ref="O26:P26"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.15748031496062992" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="78" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7165,8 +7254,8 @@
   </sheetPr>
   <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P57" sqref="P57"/>
+    <sheetView topLeftCell="G17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -7193,10 +7282,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="706" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="706"/>
+      <c r="B1" s="715" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="715"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -7214,26 +7303,26 @@
         <v>45201</v>
       </c>
       <c r="C2" s="570"/>
-      <c r="F2" s="681" t="s">
+      <c r="F2" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="682"/>
-      <c r="H2" s="683"/>
-      <c r="I2" s="684"/>
-      <c r="J2" s="685" t="s">
+      <c r="G2" s="691"/>
+      <c r="H2" s="692"/>
+      <c r="I2" s="693"/>
+      <c r="J2" s="694" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="685"/>
-      <c r="L2" s="686"/>
+      <c r="K2" s="694"/>
+      <c r="L2" s="695"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="703" t="s">
+      <c r="N2" s="712" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="703"/>
-      <c r="P2" s="712" t="s">
+      <c r="O2" s="712"/>
+      <c r="P2" s="726" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="713"/>
+      <c r="Q2" s="727"/>
       <c r="S2" s="12"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
@@ -7241,27 +7330,27 @@
     </row>
     <row r="3" spans="2:26" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="568"/>
-      <c r="C3" s="707" t="s">
+      <c r="C3" s="716" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="690"/>
+      <c r="D3" s="699"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="691" t="s">
+      <c r="F3" s="700" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="692"/>
+      <c r="G3" s="701"/>
       <c r="H3" s="586"/>
-      <c r="I3" s="716" t="s">
+      <c r="I3" s="730" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="687"/>
-      <c r="K3" s="687"/>
-      <c r="L3" s="688"/>
+      <c r="J3" s="696"/>
+      <c r="K3" s="696"/>
+      <c r="L3" s="697"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="703"/>
-      <c r="O3" s="703"/>
-      <c r="P3" s="714"/>
-      <c r="Q3" s="715"/>
+      <c r="N3" s="712"/>
+      <c r="O3" s="712"/>
+      <c r="P3" s="728"/>
+      <c r="Q3" s="729"/>
       <c r="R3" s="434"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
@@ -7288,7 +7377,7 @@
       <c r="H4" s="587" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="717"/>
+      <c r="I4" s="731"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -7749,10 +7838,10 @@
         <v>24</v>
       </c>
       <c r="M14" s="526"/>
-      <c r="N14" s="723">
+      <c r="N14" s="732">
         <v>744.11</v>
       </c>
-      <c r="O14" s="725">
+      <c r="O14" s="734">
         <v>24</v>
       </c>
       <c r="P14" s="562">
@@ -7764,7 +7853,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="411"/>
-      <c r="S14" s="722"/>
+      <c r="S14" s="725"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
@@ -7790,8 +7879,8 @@
       <c r="K15" s="524"/>
       <c r="L15" s="525"/>
       <c r="M15" s="526"/>
-      <c r="N15" s="724"/>
-      <c r="O15" s="726"/>
+      <c r="N15" s="733"/>
+      <c r="O15" s="735"/>
       <c r="P15" s="562">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -7801,7 +7890,7 @@
         <v>0</v>
       </c>
       <c r="R15" s="412"/>
-      <c r="S15" s="722"/>
+      <c r="S15" s="725"/>
       <c r="T15" s="13"/>
       <c r="U15" s="13"/>
       <c r="V15" s="13"/>
@@ -8014,7 +8103,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="413"/>
-      <c r="S20" s="722"/>
+      <c r="S20" s="725"/>
       <c r="T20" s="77"/>
       <c r="U20" s="77"/>
       <c r="V20" s="13"/>
@@ -8051,7 +8140,7 @@
         <v>0</v>
       </c>
       <c r="R21" s="623"/>
-      <c r="S21" s="722"/>
+      <c r="S21" s="725"/>
       <c r="T21" s="78"/>
       <c r="U21" s="78"/>
       <c r="V21" s="13"/>
@@ -8100,7 +8189,7 @@
         <v>0</v>
       </c>
       <c r="R22" s="624"/>
-      <c r="S22" s="722"/>
+      <c r="S22" s="725"/>
       <c r="T22" s="13"/>
       <c r="U22" s="13"/>
       <c r="V22" s="13"/>
@@ -8137,7 +8226,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="414"/>
-      <c r="S23" s="722"/>
+      <c r="S23" s="725"/>
       <c r="T23" s="13"/>
       <c r="U23" s="13"/>
       <c r="V23" s="13"/>
@@ -9208,10 +9297,10 @@
     <row r="50" spans="2:22" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" s="145"/>
       <c r="D50" s="147"/>
-      <c r="F50" s="695" t="s">
+      <c r="F50" s="704" t="s">
         <v>46</v>
       </c>
-      <c r="G50" s="695"/>
+      <c r="G50" s="704"/>
       <c r="H50" s="560">
         <f>SUM(H5:H33)</f>
         <v>25434.93</v>
@@ -9432,6 +9521,2306 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:Z62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="146" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="156" customWidth="1"/>
+    <col min="16" max="16" width="13" style="161" customWidth="1"/>
+    <col min="17" max="17" width="10" style="146" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5703125" style="109" customWidth="1"/>
+    <col min="19" max="19" width="46.28515625" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="715" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="715"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="13"/>
+    </row>
+    <row r="2" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="569">
+        <v>45255</v>
+      </c>
+      <c r="C2" s="570"/>
+      <c r="F2" s="690" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="691"/>
+      <c r="H2" s="692"/>
+      <c r="I2" s="693"/>
+      <c r="J2" s="694" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="694"/>
+      <c r="L2" s="695"/>
+      <c r="M2" s="221"/>
+      <c r="N2" s="712" t="s">
+        <v>126</v>
+      </c>
+      <c r="O2" s="712"/>
+      <c r="P2" s="726" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="727"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+    </row>
+    <row r="3" spans="2:26" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="568"/>
+      <c r="C3" s="716" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="699"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="700" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="701"/>
+      <c r="H3" s="586"/>
+      <c r="I3" s="730" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="696"/>
+      <c r="K3" s="696"/>
+      <c r="L3" s="697"/>
+      <c r="M3" s="222"/>
+      <c r="N3" s="712"/>
+      <c r="O3" s="712"/>
+      <c r="P3" s="728"/>
+      <c r="Q3" s="729"/>
+      <c r="R3" s="434"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+    </row>
+    <row r="4" spans="2:26" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="587" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="731"/>
+      <c r="J4" s="235"/>
+      <c r="K4" s="236" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="237" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="222"/>
+      <c r="N4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="588" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="589" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="435"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+    </row>
+    <row r="5" spans="2:26" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="28">
+        <v>967.84</v>
+      </c>
+      <c r="G5" s="31">
+        <v>81</v>
+      </c>
+      <c r="H5" s="223">
+        <f>F5+C5</f>
+        <v>967.84</v>
+      </c>
+      <c r="I5" s="41">
+        <f>G5+D5</f>
+        <v>81</v>
+      </c>
+      <c r="J5" s="54"/>
+      <c r="K5" s="287">
+        <v>967.84</v>
+      </c>
+      <c r="L5" s="288">
+        <v>81</v>
+      </c>
+      <c r="M5" s="42"/>
+      <c r="N5" s="627"/>
+      <c r="O5" s="628"/>
+      <c r="P5" s="239">
+        <f>H5-K5</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="44">
+        <f>I5-L5</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="653"/>
+      <c r="S5" s="430"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+    </row>
+    <row r="6" spans="2:26" ht="23.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="267"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="223">
+        <f>F6+C6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="41">
+        <f>G6+D6</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="54"/>
+      <c r="K6" s="279"/>
+      <c r="L6" s="214"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="627"/>
+      <c r="O6" s="628"/>
+      <c r="P6" s="325">
+        <f>N6-K6</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="326">
+        <f>O6-L6</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="654"/>
+      <c r="S6" s="426"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="46"/>
+      <c r="V6" s="47"/>
+      <c r="W6" s="48"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="50"/>
+      <c r="Z6" s="1"/>
+    </row>
+    <row r="7" spans="2:26" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="60">
+        <v>236.53</v>
+      </c>
+      <c r="D7" s="29">
+        <v>20</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="28">
+        <v>595.49</v>
+      </c>
+      <c r="G7" s="31">
+        <v>49</v>
+      </c>
+      <c r="H7" s="223">
+        <f>F7+C7</f>
+        <v>832.02</v>
+      </c>
+      <c r="I7" s="41">
+        <f>G7+D7</f>
+        <v>69</v>
+      </c>
+      <c r="J7" s="54"/>
+      <c r="K7" s="279">
+        <v>832.02</v>
+      </c>
+      <c r="L7" s="214">
+        <v>69</v>
+      </c>
+      <c r="M7" s="42"/>
+      <c r="N7" s="627"/>
+      <c r="O7" s="628"/>
+      <c r="P7" s="325">
+        <f t="shared" ref="P7:Q9" si="0">N7-K7</f>
+        <v>-832.02</v>
+      </c>
+      <c r="Q7" s="326">
+        <f t="shared" si="0"/>
+        <v>-69</v>
+      </c>
+      <c r="R7" s="53"/>
+      <c r="S7" s="426"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+    </row>
+    <row r="8" spans="2:26" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="514" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="224">
+        <f>F8+C8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="225">
+        <f>G8+D8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="54"/>
+      <c r="K8" s="279"/>
+      <c r="L8" s="214"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="627"/>
+      <c r="O8" s="628"/>
+      <c r="P8" s="325">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="326">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="655"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+    </row>
+    <row r="9" spans="2:26" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="514" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="28">
+        <v>167.58</v>
+      </c>
+      <c r="D9" s="29">
+        <v>9</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="639"/>
+      <c r="G9" s="640"/>
+      <c r="H9" s="224">
+        <f>F9+C9</f>
+        <v>167.58</v>
+      </c>
+      <c r="I9" s="225">
+        <f>G9+D9</f>
+        <v>9</v>
+      </c>
+      <c r="J9" s="54"/>
+      <c r="K9" s="279">
+        <v>167.58</v>
+      </c>
+      <c r="L9" s="214">
+        <v>9</v>
+      </c>
+      <c r="M9" s="42"/>
+      <c r="N9" s="627"/>
+      <c r="O9" s="628"/>
+      <c r="P9" s="325">
+        <f t="shared" si="0"/>
+        <v>-167.58</v>
+      </c>
+      <c r="Q9" s="326">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="R9" s="655"/>
+      <c r="S9" s="603"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+    </row>
+    <row r="10" spans="2:26" ht="22.5" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="514" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="193"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="226">
+        <f>F10+C10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="225">
+        <f>G10+D10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="54"/>
+      <c r="K10" s="598"/>
+      <c r="L10" s="599"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="627"/>
+      <c r="O10" s="628"/>
+      <c r="P10" s="327">
+        <f t="shared" ref="P10:Q50" si="1">H10-K10</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="448">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="410"/>
+      <c r="S10" s="604"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+    </row>
+    <row r="11" spans="2:26" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="514" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="28">
+        <v>90</v>
+      </c>
+      <c r="G11" s="31">
+        <v>9</v>
+      </c>
+      <c r="H11" s="535">
+        <f>F11+C11</f>
+        <v>90</v>
+      </c>
+      <c r="I11" s="522">
+        <f>G11+D11</f>
+        <v>9</v>
+      </c>
+      <c r="J11" s="523"/>
+      <c r="K11" s="524">
+        <v>90</v>
+      </c>
+      <c r="L11" s="525">
+        <v>9</v>
+      </c>
+      <c r="M11" s="42"/>
+      <c r="N11" s="627"/>
+      <c r="O11" s="628"/>
+      <c r="P11" s="327"/>
+      <c r="Q11" s="448"/>
+      <c r="R11" s="410"/>
+      <c r="S11" s="617"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+    </row>
+    <row r="12" spans="2:26" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="514" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="60"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="60">
+        <v>130</v>
+      </c>
+      <c r="G12" s="31">
+        <v>13</v>
+      </c>
+      <c r="H12" s="521">
+        <f>F12+C12</f>
+        <v>130</v>
+      </c>
+      <c r="I12" s="522">
+        <f>G12+D12</f>
+        <v>13</v>
+      </c>
+      <c r="J12" s="523"/>
+      <c r="K12" s="524">
+        <v>130</v>
+      </c>
+      <c r="L12" s="525">
+        <v>13</v>
+      </c>
+      <c r="M12" s="526"/>
+      <c r="N12" s="627"/>
+      <c r="O12" s="628"/>
+      <c r="P12" s="327">
+        <f>N12-H12</f>
+        <v>-130</v>
+      </c>
+      <c r="Q12" s="328">
+        <f>O12-I12</f>
+        <v>-13</v>
+      </c>
+      <c r="R12" s="656"/>
+      <c r="S12" s="605"/>
+      <c r="T12" s="66"/>
+      <c r="U12" s="66"/>
+      <c r="V12" s="13"/>
+    </row>
+    <row r="13" spans="2:26" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="515" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="28">
+        <v>1022.39</v>
+      </c>
+      <c r="G13" s="31">
+        <v>42</v>
+      </c>
+      <c r="H13" s="521">
+        <f>F13+C13</f>
+        <v>1022.39</v>
+      </c>
+      <c r="I13" s="522">
+        <f>G13+D13</f>
+        <v>42</v>
+      </c>
+      <c r="J13" s="523"/>
+      <c r="K13" s="739">
+        <v>1719.97</v>
+      </c>
+      <c r="L13" s="740">
+        <v>67</v>
+      </c>
+      <c r="M13" s="526"/>
+      <c r="N13" s="627"/>
+      <c r="O13" s="628"/>
+      <c r="P13" s="562">
+        <f t="shared" ref="P13:Q40" si="2">N13-H13</f>
+        <v>-1022.39</v>
+      </c>
+      <c r="Q13" s="448">
+        <f t="shared" si="2"/>
+        <v>-42</v>
+      </c>
+      <c r="R13" s="411"/>
+      <c r="S13" s="742" t="s">
+        <v>163</v>
+      </c>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+    </row>
+    <row r="14" spans="2:26" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="515" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="28">
+        <v>697.58</v>
+      </c>
+      <c r="G14" s="31">
+        <v>24</v>
+      </c>
+      <c r="H14" s="521">
+        <f>F14+C14</f>
+        <v>697.58</v>
+      </c>
+      <c r="I14" s="522">
+        <f>G14+D14</f>
+        <v>24</v>
+      </c>
+      <c r="J14" s="523"/>
+      <c r="K14" s="741">
+        <v>0</v>
+      </c>
+      <c r="L14" s="740">
+        <v>0</v>
+      </c>
+      <c r="M14" s="526"/>
+      <c r="N14" s="627"/>
+      <c r="O14" s="628"/>
+      <c r="P14" s="562">
+        <f t="shared" si="2"/>
+        <v>-697.58</v>
+      </c>
+      <c r="Q14" s="448">
+        <f t="shared" si="2"/>
+        <v>-24</v>
+      </c>
+      <c r="R14" s="412"/>
+      <c r="S14" s="742"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+    </row>
+    <row r="15" spans="2:26" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="514" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="521">
+        <f>F15+C15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="522">
+        <f>G15+D15</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="523"/>
+      <c r="K15" s="524"/>
+      <c r="L15" s="525"/>
+      <c r="M15" s="526"/>
+      <c r="N15" s="627"/>
+      <c r="O15" s="628"/>
+      <c r="P15" s="563">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="564">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="412"/>
+      <c r="S15" s="607"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+    </row>
+    <row r="16" spans="2:26" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="506" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="508"/>
+      <c r="D16" s="509"/>
+      <c r="E16" s="507"/>
+      <c r="F16" s="641">
+        <v>1054.58</v>
+      </c>
+      <c r="G16" s="642">
+        <v>47</v>
+      </c>
+      <c r="H16" s="583">
+        <f>F16+C16</f>
+        <v>1054.58</v>
+      </c>
+      <c r="I16" s="584">
+        <f>G16+D16</f>
+        <v>47</v>
+      </c>
+      <c r="J16" s="523"/>
+      <c r="K16" s="524">
+        <v>1054.58</v>
+      </c>
+      <c r="L16" s="525">
+        <v>47</v>
+      </c>
+      <c r="M16" s="526"/>
+      <c r="N16" s="627"/>
+      <c r="O16" s="628"/>
+      <c r="P16" s="566">
+        <f t="shared" si="2"/>
+        <v>-1054.58</v>
+      </c>
+      <c r="Q16" s="567">
+        <f t="shared" si="2"/>
+        <v>-47</v>
+      </c>
+      <c r="R16" s="436"/>
+      <c r="S16" s="661"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+    </row>
+    <row r="17" spans="2:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="514" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="28">
+        <v>374.77</v>
+      </c>
+      <c r="G17" s="31">
+        <v>12</v>
+      </c>
+      <c r="H17" s="521">
+        <f>F17+C17</f>
+        <v>374.77</v>
+      </c>
+      <c r="I17" s="522">
+        <f>G17+D17</f>
+        <v>12</v>
+      </c>
+      <c r="J17" s="523"/>
+      <c r="K17" s="524">
+        <v>374.77</v>
+      </c>
+      <c r="L17" s="525">
+        <v>12</v>
+      </c>
+      <c r="M17" s="526"/>
+      <c r="N17" s="627"/>
+      <c r="O17" s="628"/>
+      <c r="P17" s="585">
+        <f t="shared" si="2"/>
+        <v>-374.77</v>
+      </c>
+      <c r="Q17" s="326">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+      <c r="R17" s="437"/>
+      <c r="S17" s="608"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+    </row>
+    <row r="18" spans="2:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="736" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="28">
+        <v>806.98</v>
+      </c>
+      <c r="G18" s="31">
+        <v>30</v>
+      </c>
+      <c r="H18" s="521">
+        <f>F18+C18</f>
+        <v>806.98</v>
+      </c>
+      <c r="I18" s="522">
+        <f>G18+D18</f>
+        <v>30</v>
+      </c>
+      <c r="J18" s="523"/>
+      <c r="K18" s="524">
+        <v>806.98</v>
+      </c>
+      <c r="L18" s="525">
+        <v>30</v>
+      </c>
+      <c r="M18" s="526"/>
+      <c r="N18" s="627"/>
+      <c r="O18" s="628"/>
+      <c r="P18" s="585">
+        <f t="shared" ref="P18:P19" si="3">N18-H18</f>
+        <v>-806.98</v>
+      </c>
+      <c r="Q18" s="326">
+        <f t="shared" ref="Q18:Q19" si="4">O18-I18</f>
+        <v>-30</v>
+      </c>
+      <c r="R18" s="437"/>
+      <c r="S18" s="608"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+    </row>
+    <row r="19" spans="2:22" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="738" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="28">
+        <v>737.87</v>
+      </c>
+      <c r="G19" s="31">
+        <v>28</v>
+      </c>
+      <c r="H19" s="521">
+        <f>F19+C19</f>
+        <v>737.87</v>
+      </c>
+      <c r="I19" s="522">
+        <f>G19+D19</f>
+        <v>28</v>
+      </c>
+      <c r="J19" s="523"/>
+      <c r="K19" s="524">
+        <v>737.87</v>
+      </c>
+      <c r="L19" s="525">
+        <v>28</v>
+      </c>
+      <c r="M19" s="526"/>
+      <c r="N19" s="627"/>
+      <c r="O19" s="628"/>
+      <c r="P19" s="585">
+        <f t="shared" si="3"/>
+        <v>-737.87</v>
+      </c>
+      <c r="Q19" s="326">
+        <f t="shared" si="4"/>
+        <v>-28</v>
+      </c>
+      <c r="R19" s="657"/>
+      <c r="S19" s="607"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+    </row>
+    <row r="20" spans="2:22" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="514" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="28">
+        <v>1862.88</v>
+      </c>
+      <c r="G20" s="31">
+        <v>78</v>
+      </c>
+      <c r="H20" s="521">
+        <f>F20+C20</f>
+        <v>1862.88</v>
+      </c>
+      <c r="I20" s="522">
+        <f>G20+D20</f>
+        <v>78</v>
+      </c>
+      <c r="J20" s="523"/>
+      <c r="K20" s="524">
+        <v>1862.97</v>
+      </c>
+      <c r="L20" s="525">
+        <v>78</v>
+      </c>
+      <c r="M20" s="526"/>
+      <c r="N20" s="627"/>
+      <c r="O20" s="628"/>
+      <c r="P20" s="585">
+        <f t="shared" ref="P20:P21" si="5">N20-H20</f>
+        <v>-1862.88</v>
+      </c>
+      <c r="Q20" s="326">
+        <f t="shared" ref="Q20:Q21" si="6">O20-I20</f>
+        <v>-78</v>
+      </c>
+      <c r="R20" s="657"/>
+      <c r="S20" s="607"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+    </row>
+    <row r="21" spans="2:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="514" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="521">
+        <f>F21+C21</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="522">
+        <f>G21+D21</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="523"/>
+      <c r="K21" s="524"/>
+      <c r="L21" s="525"/>
+      <c r="M21" s="526"/>
+      <c r="N21" s="627"/>
+      <c r="O21" s="628"/>
+      <c r="P21" s="585">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="326">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="413"/>
+      <c r="S21" s="725"/>
+      <c r="T21" s="77"/>
+      <c r="U21" s="77"/>
+      <c r="V21" s="13"/>
+    </row>
+    <row r="22" spans="2:22" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="514" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="28">
+        <v>300.44</v>
+      </c>
+      <c r="G22" s="31">
+        <v>12</v>
+      </c>
+      <c r="H22" s="521">
+        <f>F22+C22</f>
+        <v>300.44</v>
+      </c>
+      <c r="I22" s="522">
+        <f>G22+D22</f>
+        <v>12</v>
+      </c>
+      <c r="J22" s="523"/>
+      <c r="K22" s="524">
+        <v>300.44</v>
+      </c>
+      <c r="L22" s="525">
+        <v>12</v>
+      </c>
+      <c r="M22" s="526"/>
+      <c r="N22" s="627"/>
+      <c r="O22" s="628"/>
+      <c r="P22" s="327">
+        <f t="shared" si="2"/>
+        <v>-300.44</v>
+      </c>
+      <c r="Q22" s="328">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+      <c r="R22" s="658"/>
+      <c r="S22" s="725"/>
+      <c r="T22" s="78"/>
+      <c r="U22" s="78"/>
+      <c r="V22" s="13"/>
+    </row>
+    <row r="23" spans="2:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="514" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="28">
+        <v>1405.89</v>
+      </c>
+      <c r="G23" s="31">
+        <v>82</v>
+      </c>
+      <c r="H23" s="521">
+        <f>F23+C23</f>
+        <v>1405.89</v>
+      </c>
+      <c r="I23" s="522">
+        <f>G23+D23</f>
+        <v>82</v>
+      </c>
+      <c r="J23" s="523"/>
+      <c r="K23" s="741">
+        <v>1458.4</v>
+      </c>
+      <c r="L23" s="740">
+        <v>85</v>
+      </c>
+      <c r="M23" s="526"/>
+      <c r="N23" s="627"/>
+      <c r="O23" s="628"/>
+      <c r="P23" s="327"/>
+      <c r="Q23" s="328">
+        <f t="shared" si="2"/>
+        <v>-82</v>
+      </c>
+      <c r="R23" s="659"/>
+      <c r="S23" s="742" t="s">
+        <v>164</v>
+      </c>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+    </row>
+    <row r="24" spans="2:22" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="514" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="521">
+        <f>F24+C24</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="522">
+        <f>G24+D24</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="523"/>
+      <c r="K24" s="524"/>
+      <c r="L24" s="525"/>
+      <c r="M24" s="526"/>
+      <c r="N24" s="627"/>
+      <c r="O24" s="628"/>
+      <c r="P24" s="327">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="328">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="414"/>
+      <c r="S24" s="742"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+    </row>
+    <row r="25" spans="2:22" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="514" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="28">
+        <v>2674.06</v>
+      </c>
+      <c r="G25" s="31">
+        <v>589</v>
+      </c>
+      <c r="H25" s="521">
+        <f>F25+C25</f>
+        <v>2674.06</v>
+      </c>
+      <c r="I25" s="522">
+        <f>G25+D25</f>
+        <v>589</v>
+      </c>
+      <c r="J25" s="523"/>
+      <c r="K25" s="524">
+        <v>2674.55</v>
+      </c>
+      <c r="L25" s="525">
+        <v>589</v>
+      </c>
+      <c r="M25" s="526"/>
+      <c r="N25" s="627"/>
+      <c r="O25" s="628"/>
+      <c r="P25" s="327">
+        <f t="shared" si="2"/>
+        <v>-2674.06</v>
+      </c>
+      <c r="Q25" s="328">
+        <f t="shared" si="2"/>
+        <v>-589</v>
+      </c>
+      <c r="R25" s="438"/>
+      <c r="S25" s="609"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+    </row>
+    <row r="26" spans="2:22" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="514" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="115"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="28">
+        <v>241.18</v>
+      </c>
+      <c r="G26" s="31">
+        <v>9</v>
+      </c>
+      <c r="H26" s="521">
+        <f>F26+C26</f>
+        <v>241.18</v>
+      </c>
+      <c r="I26" s="522">
+        <f>G26+D26</f>
+        <v>9</v>
+      </c>
+      <c r="J26" s="523"/>
+      <c r="K26" s="524">
+        <v>241.18</v>
+      </c>
+      <c r="L26" s="525">
+        <v>9</v>
+      </c>
+      <c r="M26" s="526"/>
+      <c r="N26" s="627"/>
+      <c r="O26" s="628"/>
+      <c r="P26" s="327">
+        <f t="shared" si="2"/>
+        <v>-241.18</v>
+      </c>
+      <c r="Q26" s="328">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="R26" s="660"/>
+      <c r="S26" s="610"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
+    </row>
+    <row r="27" spans="2:22" ht="29.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="514" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="115"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="521">
+        <f>F27+C27</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="522">
+        <f>G27+D27</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="523"/>
+      <c r="K27" s="524"/>
+      <c r="L27" s="525"/>
+      <c r="M27" s="526"/>
+      <c r="N27" s="627"/>
+      <c r="O27" s="628"/>
+      <c r="P27" s="327">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="328">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="211"/>
+      <c r="S27" s="605"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+    </row>
+    <row r="28" spans="2:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="515" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="115"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="87">
+        <v>16793.16</v>
+      </c>
+      <c r="G28" s="88">
+        <v>644</v>
+      </c>
+      <c r="H28" s="521">
+        <f>F28+C28</f>
+        <v>16793.16</v>
+      </c>
+      <c r="I28" s="522">
+        <f>G28+D28</f>
+        <v>644</v>
+      </c>
+      <c r="J28" s="523"/>
+      <c r="K28" s="524">
+        <v>16793.22</v>
+      </c>
+      <c r="L28" s="525">
+        <v>644</v>
+      </c>
+      <c r="M28" s="526"/>
+      <c r="N28" s="627"/>
+      <c r="O28" s="628"/>
+      <c r="P28" s="327">
+        <f t="shared" si="2"/>
+        <v>-16793.16</v>
+      </c>
+      <c r="Q28" s="328">
+        <f t="shared" si="2"/>
+        <v>-644</v>
+      </c>
+      <c r="R28" s="211"/>
+      <c r="S28" s="611"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+    </row>
+    <row r="29" spans="2:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="514" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="115"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="88"/>
+      <c r="H29" s="521">
+        <f>F29+C29</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="522">
+        <f>G29+D29</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="523"/>
+      <c r="K29" s="524"/>
+      <c r="L29" s="525"/>
+      <c r="M29" s="526"/>
+      <c r="N29" s="627"/>
+      <c r="O29" s="628"/>
+      <c r="P29" s="327">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="328">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="211"/>
+      <c r="S29" s="605"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
+    </row>
+    <row r="30" spans="2:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="514" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="115"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="88"/>
+      <c r="H30" s="521">
+        <f>F30+C30</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="522">
+        <f>G30+D30</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="523"/>
+      <c r="K30" s="524"/>
+      <c r="L30" s="525"/>
+      <c r="M30" s="526"/>
+      <c r="N30" s="627"/>
+      <c r="O30" s="628"/>
+      <c r="P30" s="327">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="328">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R30" s="415"/>
+      <c r="S30" s="610"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+    </row>
+    <row r="31" spans="2:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="514" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="115"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="87">
+        <v>6259.29</v>
+      </c>
+      <c r="G31" s="88">
+        <v>230</v>
+      </c>
+      <c r="H31" s="535">
+        <f>F31+C31</f>
+        <v>6259.29</v>
+      </c>
+      <c r="I31" s="536">
+        <f>G31+D31</f>
+        <v>230</v>
+      </c>
+      <c r="J31" s="523"/>
+      <c r="K31" s="741">
+        <v>6259.29</v>
+      </c>
+      <c r="L31" s="740">
+        <v>229</v>
+      </c>
+      <c r="M31" s="526"/>
+      <c r="N31" s="627"/>
+      <c r="O31" s="628"/>
+      <c r="P31" s="327">
+        <f t="shared" si="2"/>
+        <v>-6259.29</v>
+      </c>
+      <c r="Q31" s="328">
+        <f t="shared" si="2"/>
+        <v>-230</v>
+      </c>
+      <c r="R31" s="656"/>
+      <c r="S31" s="743" t="s">
+        <v>165</v>
+      </c>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+    </row>
+    <row r="32" spans="2:22" ht="29.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="592" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="115"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="88"/>
+      <c r="H32" s="535">
+        <f>F32+C32</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="536">
+        <f>G32+D32</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="523"/>
+      <c r="K32" s="524"/>
+      <c r="L32" s="525"/>
+      <c r="M32" s="526"/>
+      <c r="N32" s="627"/>
+      <c r="O32" s="628"/>
+      <c r="P32" s="327">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="328">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R32" s="656"/>
+      <c r="S32" s="613"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+    </row>
+    <row r="33" spans="1:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="514" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="115">
+        <v>4020</v>
+      </c>
+      <c r="D33" s="29">
+        <v>402</v>
+      </c>
+      <c r="E33" s="30"/>
+      <c r="F33" s="87"/>
+      <c r="G33" s="88"/>
+      <c r="H33" s="535">
+        <f>F33+C33</f>
+        <v>4020</v>
+      </c>
+      <c r="I33" s="536">
+        <f>G33+D33</f>
+        <v>402</v>
+      </c>
+      <c r="J33" s="523"/>
+      <c r="K33" s="524">
+        <v>4020</v>
+      </c>
+      <c r="L33" s="525">
+        <v>402</v>
+      </c>
+      <c r="M33" s="526"/>
+      <c r="N33" s="627"/>
+      <c r="O33" s="628"/>
+      <c r="P33" s="327">
+        <f t="shared" si="2"/>
+        <v>-4020</v>
+      </c>
+      <c r="Q33" s="328">
+        <f t="shared" si="2"/>
+        <v>-402</v>
+      </c>
+      <c r="R33" s="416"/>
+      <c r="S33" s="605"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+    </row>
+    <row r="34" spans="1:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="514" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="255">
+        <v>1020</v>
+      </c>
+      <c r="D34" s="97">
+        <v>102</v>
+      </c>
+      <c r="E34" s="98"/>
+      <c r="F34" s="96"/>
+      <c r="G34" s="103"/>
+      <c r="H34" s="535">
+        <f>F34+C34</f>
+        <v>1020</v>
+      </c>
+      <c r="I34" s="536">
+        <f>G34+D34</f>
+        <v>102</v>
+      </c>
+      <c r="J34" s="523"/>
+      <c r="K34" s="524">
+        <v>1020</v>
+      </c>
+      <c r="L34" s="525">
+        <v>102</v>
+      </c>
+      <c r="M34" s="526"/>
+      <c r="N34" s="627"/>
+      <c r="O34" s="628"/>
+      <c r="P34" s="327">
+        <f t="shared" si="2"/>
+        <v>-1020</v>
+      </c>
+      <c r="Q34" s="328">
+        <f t="shared" si="2"/>
+        <v>-102</v>
+      </c>
+      <c r="R34" s="417"/>
+      <c r="S34" s="605"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+    </row>
+    <row r="35" spans="1:22" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="514" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="255"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="102"/>
+      <c r="F35" s="96">
+        <v>16632.23</v>
+      </c>
+      <c r="G35" s="103">
+        <v>676</v>
+      </c>
+      <c r="H35" s="535">
+        <f>F35+C35</f>
+        <v>16632.23</v>
+      </c>
+      <c r="I35" s="536">
+        <f>G35+D35</f>
+        <v>676</v>
+      </c>
+      <c r="J35" s="523"/>
+      <c r="K35" s="524">
+        <v>16632.23</v>
+      </c>
+      <c r="L35" s="525">
+        <v>676</v>
+      </c>
+      <c r="M35" s="526"/>
+      <c r="N35" s="627"/>
+      <c r="O35" s="628"/>
+      <c r="P35" s="327">
+        <f t="shared" si="2"/>
+        <v>-16632.23</v>
+      </c>
+      <c r="Q35" s="328">
+        <f t="shared" si="2"/>
+        <v>-676</v>
+      </c>
+      <c r="R35" s="418"/>
+      <c r="S35" s="605"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="13"/>
+    </row>
+    <row r="36" spans="1:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="514" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="255"/>
+      <c r="D36" s="97"/>
+      <c r="E36" s="102"/>
+      <c r="F36" s="96"/>
+      <c r="G36" s="103"/>
+      <c r="H36" s="535">
+        <f>F36+C36</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="536">
+        <f>G36+D36</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="523"/>
+      <c r="K36" s="524"/>
+      <c r="L36" s="525"/>
+      <c r="M36" s="526"/>
+      <c r="N36" s="627"/>
+      <c r="O36" s="628"/>
+      <c r="P36" s="327">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="328">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R36" s="418"/>
+      <c r="S36" s="614"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+    </row>
+    <row r="37" spans="1:22" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="514" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="115"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="102"/>
+      <c r="F37" s="96">
+        <v>1470</v>
+      </c>
+      <c r="G37" s="103">
+        <v>98</v>
+      </c>
+      <c r="H37" s="535">
+        <f>F37+C37</f>
+        <v>1470</v>
+      </c>
+      <c r="I37" s="536">
+        <f>G37+D37</f>
+        <v>98</v>
+      </c>
+      <c r="J37" s="523"/>
+      <c r="K37" s="524">
+        <v>1470</v>
+      </c>
+      <c r="L37" s="525">
+        <v>98</v>
+      </c>
+      <c r="M37" s="526"/>
+      <c r="N37" s="627"/>
+      <c r="O37" s="628"/>
+      <c r="P37" s="327">
+        <f t="shared" si="2"/>
+        <v>-1470</v>
+      </c>
+      <c r="Q37" s="328">
+        <f t="shared" si="2"/>
+        <v>-98</v>
+      </c>
+      <c r="R37" s="658"/>
+      <c r="S37" s="605"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
+    </row>
+    <row r="38" spans="1:22" ht="29.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="109"/>
+      <c r="B38" s="515" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="115"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="102"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="535">
+        <f>F38+C38</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="536">
+        <f>G38+D38</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="523"/>
+      <c r="K38" s="524"/>
+      <c r="L38" s="525"/>
+      <c r="M38" s="526"/>
+      <c r="N38" s="627"/>
+      <c r="O38" s="628"/>
+      <c r="P38" s="327">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="328">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R38" s="658"/>
+      <c r="S38" s="615"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+    </row>
+    <row r="39" spans="1:22" ht="39" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="737" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="115"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="102"/>
+      <c r="F39" s="96"/>
+      <c r="G39" s="103"/>
+      <c r="H39" s="537">
+        <f>F39+C39</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="538">
+        <f>G39+D39</f>
+        <v>0</v>
+      </c>
+      <c r="J39" s="523"/>
+      <c r="K39" s="524"/>
+      <c r="L39" s="525"/>
+      <c r="M39" s="526"/>
+      <c r="N39" s="627"/>
+      <c r="O39" s="628"/>
+      <c r="P39" s="327">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="328">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R39" s="114"/>
+      <c r="S39" s="616"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="13"/>
+    </row>
+    <row r="40" spans="1:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="505" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="115"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="102"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="103"/>
+      <c r="H40" s="537">
+        <f>F40+C40</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="538">
+        <f>G40+D40</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="523"/>
+      <c r="K40" s="524"/>
+      <c r="L40" s="525"/>
+      <c r="M40" s="526"/>
+      <c r="N40" s="627"/>
+      <c r="O40" s="628"/>
+      <c r="P40" s="327">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="328">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R40" s="419"/>
+      <c r="S40" s="617"/>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+      <c r="V40" s="13"/>
+    </row>
+    <row r="41" spans="1:22" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="514" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="255">
+        <v>413.95</v>
+      </c>
+      <c r="D41" s="97">
+        <v>16</v>
+      </c>
+      <c r="E41" s="102"/>
+      <c r="F41" s="96"/>
+      <c r="G41" s="258"/>
+      <c r="H41" s="539">
+        <f>F41+C41</f>
+        <v>413.95</v>
+      </c>
+      <c r="I41" s="538">
+        <f>G41+D41</f>
+        <v>16</v>
+      </c>
+      <c r="J41" s="523"/>
+      <c r="K41" s="540">
+        <v>413.95</v>
+      </c>
+      <c r="L41" s="541">
+        <v>16</v>
+      </c>
+      <c r="M41" s="526"/>
+      <c r="N41" s="627"/>
+      <c r="O41" s="628"/>
+      <c r="P41" s="327">
+        <f t="shared" ref="P41:Q44" si="7">H41-K41</f>
+        <v>0</v>
+      </c>
+      <c r="Q41" s="328">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R41" s="419"/>
+      <c r="S41" s="605"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+    </row>
+    <row r="42" spans="1:22" ht="45.75" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="514" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="255"/>
+      <c r="D42" s="97"/>
+      <c r="E42" s="111"/>
+      <c r="F42" s="96"/>
+      <c r="G42" s="258"/>
+      <c r="H42" s="539">
+        <f>F42+C42</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="538">
+        <f>G42+D42</f>
+        <v>0</v>
+      </c>
+      <c r="J42" s="542"/>
+      <c r="K42" s="543"/>
+      <c r="L42" s="544"/>
+      <c r="M42" s="542"/>
+      <c r="N42" s="627"/>
+      <c r="O42" s="628"/>
+      <c r="P42" s="327">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q42" s="328">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R42" s="420"/>
+      <c r="S42" s="605"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
+    </row>
+    <row r="43" spans="1:22" ht="45.75" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="515" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="115"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="259"/>
+      <c r="H43" s="539">
+        <f>F43+C43</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="538">
+        <f>G43+D43</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="523"/>
+      <c r="K43" s="543"/>
+      <c r="L43" s="544"/>
+      <c r="M43" s="542"/>
+      <c r="N43" s="627"/>
+      <c r="O43" s="628"/>
+      <c r="P43" s="327">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q43" s="328">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R43" s="658"/>
+      <c r="S43" s="605"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+    </row>
+    <row r="44" spans="1:22" ht="45.75" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="515" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="115"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="259"/>
+      <c r="H44" s="539">
+        <f>F44+C44</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="538">
+        <f>G44+D44</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="523"/>
+      <c r="K44" s="543"/>
+      <c r="L44" s="544"/>
+      <c r="M44" s="542"/>
+      <c r="N44" s="627"/>
+      <c r="O44" s="628"/>
+      <c r="P44" s="327">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="328">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R44" s="658"/>
+      <c r="S44" s="605"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="13"/>
+      <c r="V44" s="13"/>
+    </row>
+    <row r="45" spans="1:22" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="514" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="115"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="28">
+        <v>176.44</v>
+      </c>
+      <c r="G45" s="259">
+        <v>6</v>
+      </c>
+      <c r="H45" s="539">
+        <f>F45+C45</f>
+        <v>176.44</v>
+      </c>
+      <c r="I45" s="538">
+        <f>G45+D45</f>
+        <v>6</v>
+      </c>
+      <c r="J45" s="523"/>
+      <c r="K45" s="543">
+        <v>176.35</v>
+      </c>
+      <c r="L45" s="544">
+        <v>6</v>
+      </c>
+      <c r="M45" s="542"/>
+      <c r="N45" s="627"/>
+      <c r="O45" s="628"/>
+      <c r="P45" s="327">
+        <f>N45-H45</f>
+        <v>-176.44</v>
+      </c>
+      <c r="Q45" s="328">
+        <f>O45-I45</f>
+        <v>-6</v>
+      </c>
+      <c r="R45" s="658"/>
+      <c r="S45" s="605"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
+    </row>
+    <row r="46" spans="1:22" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="519" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" s="375"/>
+      <c r="D46" s="374"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="28">
+        <v>1175.79</v>
+      </c>
+      <c r="G46" s="259">
+        <v>46</v>
+      </c>
+      <c r="H46" s="539">
+        <f>F46+C46</f>
+        <v>1175.79</v>
+      </c>
+      <c r="I46" s="538">
+        <f>G46+D46</f>
+        <v>46</v>
+      </c>
+      <c r="J46" s="523"/>
+      <c r="K46" s="543">
+        <v>1175.79</v>
+      </c>
+      <c r="L46" s="544">
+        <v>46</v>
+      </c>
+      <c r="M46" s="542"/>
+      <c r="N46" s="627"/>
+      <c r="O46" s="628"/>
+      <c r="P46" s="327">
+        <f t="shared" ref="P46:Q47" si="8">N46-H46</f>
+        <v>-1175.79</v>
+      </c>
+      <c r="Q46" s="328">
+        <f t="shared" si="8"/>
+        <v>-46</v>
+      </c>
+      <c r="R46" s="658"/>
+      <c r="S46" s="611"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
+      <c r="V46" s="13"/>
+    </row>
+    <row r="47" spans="1:22" ht="45.75" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="519" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="115"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="259"/>
+      <c r="H47" s="539">
+        <f>F47+C47</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="538">
+        <f>G47+D47</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="523"/>
+      <c r="K47" s="543"/>
+      <c r="L47" s="544"/>
+      <c r="M47" s="542"/>
+      <c r="N47" s="631"/>
+      <c r="O47" s="632"/>
+      <c r="P47" s="327">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q47" s="328">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R47" s="658"/>
+      <c r="S47" s="605"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="13"/>
+    </row>
+    <row r="48" spans="1:22" ht="45.75" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="265" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="440"/>
+      <c r="D48" s="441"/>
+      <c r="E48" s="442"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="259"/>
+      <c r="H48" s="539">
+        <f>F48+C48</f>
+        <v>0</v>
+      </c>
+      <c r="I48" s="538">
+        <f>G48+D48</f>
+        <v>0</v>
+      </c>
+      <c r="J48" s="523"/>
+      <c r="K48" s="543"/>
+      <c r="L48" s="544"/>
+      <c r="M48" s="542"/>
+      <c r="N48" s="629"/>
+      <c r="O48" s="630"/>
+      <c r="P48" s="327">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q48" s="328">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R48" s="658"/>
+      <c r="S48" s="605"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="13"/>
+    </row>
+    <row r="49" spans="2:22" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="261"/>
+      <c r="C49" s="115"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="259"/>
+      <c r="H49" s="539">
+        <f t="shared" ref="H48:I50" si="9">F49+C49</f>
+        <v>0</v>
+      </c>
+      <c r="I49" s="538">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="523"/>
+      <c r="K49" s="543"/>
+      <c r="L49" s="544"/>
+      <c r="M49" s="542"/>
+      <c r="N49" s="629"/>
+      <c r="O49" s="630"/>
+      <c r="P49" s="327">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q49" s="328">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R49" s="658"/>
+      <c r="S49" s="605"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="13"/>
+    </row>
+    <row r="50" spans="2:22" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="266"/>
+      <c r="C50" s="269"/>
+      <c r="D50" s="271"/>
+      <c r="E50" s="273"/>
+      <c r="F50" s="275"/>
+      <c r="G50" s="277"/>
+      <c r="H50" s="539">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="538">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="523"/>
+      <c r="K50" s="543"/>
+      <c r="L50" s="544"/>
+      <c r="M50" s="542"/>
+      <c r="N50" s="246"/>
+      <c r="O50" s="247"/>
+      <c r="P50" s="329">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q50" s="330">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R50" s="143"/>
+      <c r="S50" s="45"/>
+      <c r="T50" s="13"/>
+      <c r="U50" s="13"/>
+      <c r="V50" s="13"/>
+    </row>
+    <row r="51" spans="2:22" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="145"/>
+      <c r="D51" s="147"/>
+      <c r="F51" s="704" t="s">
+        <v>46</v>
+      </c>
+      <c r="G51" s="704"/>
+      <c r="H51" s="560">
+        <f>SUM(H5:H34)</f>
+        <v>41458.51</v>
+      </c>
+      <c r="I51" s="561">
+        <f>SUM(I5:I34)</f>
+        <v>2512</v>
+      </c>
+      <c r="J51" s="149"/>
+      <c r="K51" s="149"/>
+      <c r="L51" s="149"/>
+      <c r="M51" s="150"/>
+      <c r="N51" s="559">
+        <f>SUM(N5:N42)</f>
+        <v>0</v>
+      </c>
+      <c r="O51" s="559">
+        <f>SUM(O5:O42)</f>
+        <v>0</v>
+      </c>
+      <c r="P51" s="153"/>
+      <c r="Q51" s="154"/>
+      <c r="R51" s="155"/>
+      <c r="S51" s="45"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="13"/>
+      <c r="V51" s="13"/>
+    </row>
+    <row r="52" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="P52" s="157"/>
+      <c r="Q52" s="158"/>
+      <c r="R52" s="439"/>
+      <c r="S52" s="45"/>
+      <c r="T52" s="13"/>
+      <c r="U52" s="13"/>
+      <c r="V52" s="13"/>
+    </row>
+    <row r="53" spans="2:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="77"/>
+      <c r="C53" s="160"/>
+      <c r="D53" s="77"/>
+      <c r="E53" s="77"/>
+      <c r="F53" s="77"/>
+      <c r="G53" s="1"/>
+      <c r="S53" s="12"/>
+      <c r="T53" s="13"/>
+      <c r="U53" s="13"/>
+      <c r="V53" s="13"/>
+    </row>
+    <row r="54" spans="2:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="352" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="353"/>
+      <c r="E54" s="354"/>
+      <c r="F54" s="354"/>
+      <c r="G54" s="355"/>
+      <c r="H54" s="166"/>
+      <c r="I54" s="166"/>
+      <c r="J54" s="166"/>
+      <c r="K54" s="166"/>
+      <c r="L54" s="166"/>
+      <c r="M54" s="166"/>
+      <c r="N54" s="166"/>
+      <c r="O54" s="167"/>
+      <c r="P54" s="168"/>
+      <c r="Q54" s="169"/>
+    </row>
+    <row r="55" spans="2:22" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="170"/>
+      <c r="D55" s="315"/>
+      <c r="E55" s="316"/>
+      <c r="F55" s="316"/>
+      <c r="G55" s="317"/>
+      <c r="H55" s="317"/>
+      <c r="I55" s="317"/>
+      <c r="J55" s="301"/>
+      <c r="K55" s="301"/>
+      <c r="L55" s="301"/>
+      <c r="M55" s="301"/>
+      <c r="N55" s="301"/>
+      <c r="O55" s="302"/>
+      <c r="P55" s="303"/>
+      <c r="Q55" s="304"/>
+      <c r="R55" s="174"/>
+      <c r="S55" s="173"/>
+      <c r="T55" s="174"/>
+    </row>
+    <row r="56" spans="2:22" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="175"/>
+      <c r="C56" s="176"/>
+      <c r="D56" s="177"/>
+      <c r="E56" s="77"/>
+      <c r="F56" s="77"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="13"/>
+      <c r="O56" s="178"/>
+      <c r="P56" s="179"/>
+      <c r="Q56" s="169"/>
+    </row>
+    <row r="57" spans="2:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="175"/>
+      <c r="C57" s="485"/>
+      <c r="D57" s="486"/>
+      <c r="E57" s="487"/>
+      <c r="F57" s="487"/>
+      <c r="G57" s="487"/>
+      <c r="H57" s="487"/>
+      <c r="I57" s="488"/>
+      <c r="J57" s="488"/>
+      <c r="K57" s="488"/>
+      <c r="L57" s="181"/>
+      <c r="M57" s="181"/>
+      <c r="N57" s="181"/>
+      <c r="O57" s="181"/>
+      <c r="P57" s="179"/>
+      <c r="Q57" s="169"/>
+    </row>
+    <row r="58" spans="2:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="175"/>
+      <c r="C58" s="600"/>
+      <c r="D58" s="601"/>
+      <c r="E58" s="602"/>
+      <c r="F58" s="602"/>
+      <c r="G58" s="602"/>
+      <c r="H58" s="602"/>
+      <c r="I58" s="602"/>
+      <c r="J58" s="602"/>
+      <c r="K58" s="602"/>
+      <c r="L58" s="183"/>
+      <c r="M58" s="183"/>
+      <c r="N58" s="183"/>
+      <c r="O58" s="178"/>
+      <c r="P58" s="184"/>
+      <c r="Q58" s="185"/>
+    </row>
+    <row r="59" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="175"/>
+      <c r="C59" s="176"/>
+      <c r="D59" s="186"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="178"/>
+      <c r="P59" s="184"/>
+      <c r="Q59" s="185"/>
+    </row>
+    <row r="60" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="175"/>
+      <c r="C60" s="176"/>
+      <c r="D60" s="187"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+      <c r="L60" s="13"/>
+      <c r="M60" s="13"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="178"/>
+      <c r="P60" s="184"/>
+      <c r="Q60" s="185"/>
+    </row>
+    <row r="61" spans="2:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="175"/>
+      <c r="C61" s="176"/>
+      <c r="D61" s="188"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="13"/>
+      <c r="N61" s="13"/>
+      <c r="O61" s="178"/>
+    </row>
+    <row r="62" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
+    </row>
+  </sheetData>
+  <sortState ref="B5:L49">
+    <sortCondition ref="B5:B49"/>
+  </sortState>
+  <mergeCells count="12">
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="S21:S22"/>
+    <mergeCell ref="S23:S24"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="P2:Q3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
+  </mergeCells>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.15748031496062992" header="0.21" footer="0.16"/>
+  <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9478,10 +11867,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="653" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="654"/>
+      <c r="B1" s="676" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="677"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -9496,26 +11885,26 @@
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="2:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="679">
+      <c r="B2" s="688">
         <v>44989</v>
       </c>
-      <c r="C2" s="680"/>
-      <c r="F2" s="681" t="s">
+      <c r="C2" s="689"/>
+      <c r="F2" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="682"/>
-      <c r="H2" s="683"/>
-      <c r="I2" s="684"/>
-      <c r="J2" s="685" t="s">
+      <c r="G2" s="691"/>
+      <c r="H2" s="692"/>
+      <c r="I2" s="693"/>
+      <c r="J2" s="694" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="685"/>
-      <c r="L2" s="686"/>
+      <c r="K2" s="694"/>
+      <c r="L2" s="695"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="658" t="s">
+      <c r="N2" s="681" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="658"/>
+      <c r="O2" s="681"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
       <c r="T2" s="12"/>
@@ -9525,33 +11914,33 @@
     </row>
     <row r="3" spans="2:27" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="689" t="s">
+      <c r="C3" s="698" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="690"/>
+      <c r="D3" s="699"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="691" t="s">
+      <c r="F3" s="700" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="692"/>
+      <c r="G3" s="701"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="693" t="s">
+      <c r="I3" s="702" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="687"/>
-      <c r="K3" s="687"/>
-      <c r="L3" s="688"/>
+      <c r="J3" s="696"/>
+      <c r="K3" s="696"/>
+      <c r="L3" s="697"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="658"/>
-      <c r="O3" s="658"/>
-      <c r="P3" s="666" t="s">
+      <c r="N3" s="681"/>
+      <c r="O3" s="681"/>
+      <c r="P3" s="663" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="667"/>
-      <c r="R3" s="668" t="s">
+      <c r="Q3" s="664"/>
+      <c r="R3" s="665" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="669"/>
+      <c r="S3" s="666"/>
       <c r="T3" s="12"/>
       <c r="U3" s="13"/>
       <c r="V3" s="13"/>
@@ -9577,7 +11966,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="694"/>
+      <c r="I4" s="703"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -9653,8 +12042,8 @@
       <c r="Q5" s="38">
         <v>0</v>
       </c>
-      <c r="R5" s="670"/>
-      <c r="S5" s="670"/>
+      <c r="R5" s="667"/>
+      <c r="S5" s="667"/>
       <c r="T5" s="12"/>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
@@ -9691,8 +12080,8 @@
         <f>O6-I6</f>
         <v>0</v>
       </c>
-      <c r="R6" s="671"/>
-      <c r="S6" s="671"/>
+      <c r="R6" s="668"/>
+      <c r="S6" s="668"/>
       <c r="T6" s="45"/>
       <c r="U6" s="13"/>
       <c r="V6" s="46"/>
@@ -9779,8 +12168,8 @@
       <c r="Q8" s="52">
         <v>0</v>
       </c>
-      <c r="R8" s="672"/>
-      <c r="S8" s="672"/>
+      <c r="R8" s="669"/>
+      <c r="S8" s="669"/>
       <c r="T8" s="45"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
@@ -9867,8 +12256,8 @@
       <c r="Q10" s="52">
         <v>0</v>
       </c>
-      <c r="R10" s="673"/>
-      <c r="S10" s="673"/>
+      <c r="R10" s="670"/>
+      <c r="S10" s="670"/>
       <c r="T10" s="45"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -10008,8 +12397,8 @@
       <c r="Q13" s="52">
         <v>0</v>
       </c>
-      <c r="R13" s="674"/>
-      <c r="S13" s="674"/>
+      <c r="R13" s="671"/>
+      <c r="S13" s="671"/>
       <c r="T13" s="45"/>
       <c r="U13" s="66"/>
       <c r="V13" s="66"/>
@@ -10317,8 +12706,8 @@
       <c r="Q20" s="52">
         <v>0</v>
       </c>
-      <c r="R20" s="675"/>
-      <c r="S20" s="675"/>
+      <c r="R20" s="672"/>
+      <c r="S20" s="672"/>
       <c r="T20" s="45"/>
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
@@ -10405,8 +12794,8 @@
       <c r="Q22" s="52">
         <v>0</v>
       </c>
-      <c r="R22" s="676"/>
-      <c r="S22" s="676"/>
+      <c r="R22" s="673"/>
+      <c r="S22" s="673"/>
       <c r="T22" s="45"/>
       <c r="U22" s="78"/>
       <c r="V22" s="78"/>
@@ -10452,8 +12841,8 @@
       <c r="Q23" s="52">
         <v>0</v>
       </c>
-      <c r="R23" s="677"/>
-      <c r="S23" s="677"/>
+      <c r="R23" s="674"/>
+      <c r="S23" s="674"/>
       <c r="T23" s="45"/>
       <c r="U23" s="13"/>
       <c r="V23" s="13"/>
@@ -10593,8 +12982,8 @@
       <c r="Q26" s="52">
         <v>0</v>
       </c>
-      <c r="R26" s="678"/>
-      <c r="S26" s="678"/>
+      <c r="R26" s="675"/>
+      <c r="S26" s="675"/>
       <c r="T26" s="45"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
@@ -11277,10 +13666,10 @@
     <row r="43" spans="1:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="145"/>
       <c r="D43" s="147"/>
-      <c r="F43" s="665" t="s">
+      <c r="F43" s="662" t="s">
         <v>46</v>
       </c>
-      <c r="G43" s="665"/>
+      <c r="G43" s="662"/>
       <c r="H43" s="148">
         <f>SUM(H5:H34)</f>
         <v>52842.86</v>
@@ -11501,6 +13890,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
@@ -11513,14 +13910,6 @@
     <mergeCell ref="R22:S22"/>
     <mergeCell ref="R23:S23"/>
     <mergeCell ref="R26:S26"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.35" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11563,10 +13952,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="653" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="654"/>
+      <c r="B1" s="676" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="677"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -11581,26 +13970,26 @@
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="2:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="679">
+      <c r="B2" s="688">
         <v>45017</v>
       </c>
-      <c r="C2" s="680"/>
-      <c r="F2" s="681" t="s">
+      <c r="C2" s="689"/>
+      <c r="F2" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="682"/>
-      <c r="H2" s="683"/>
-      <c r="I2" s="684"/>
-      <c r="J2" s="685" t="s">
+      <c r="G2" s="691"/>
+      <c r="H2" s="692"/>
+      <c r="I2" s="693"/>
+      <c r="J2" s="694" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="685"/>
-      <c r="L2" s="686"/>
+      <c r="K2" s="694"/>
+      <c r="L2" s="695"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="658" t="s">
+      <c r="N2" s="681" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="658"/>
+      <c r="O2" s="681"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
       <c r="T2" s="12"/>
@@ -11610,33 +13999,33 @@
     </row>
     <row r="3" spans="2:27" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="689" t="s">
+      <c r="C3" s="698" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="690"/>
+      <c r="D3" s="699"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="691" t="s">
+      <c r="F3" s="700" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="692"/>
+      <c r="G3" s="701"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="693" t="s">
+      <c r="I3" s="702" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="687"/>
-      <c r="K3" s="687"/>
-      <c r="L3" s="688"/>
+      <c r="J3" s="696"/>
+      <c r="K3" s="696"/>
+      <c r="L3" s="697"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="658"/>
-      <c r="O3" s="658"/>
-      <c r="P3" s="666" t="s">
+      <c r="N3" s="681"/>
+      <c r="O3" s="681"/>
+      <c r="P3" s="663" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="667"/>
-      <c r="R3" s="668" t="s">
+      <c r="Q3" s="664"/>
+      <c r="R3" s="665" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="669"/>
+      <c r="S3" s="666"/>
       <c r="T3" s="12"/>
       <c r="U3" s="13"/>
       <c r="V3" s="13"/>
@@ -11662,7 +14051,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="694"/>
+      <c r="I4" s="703"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -11737,8 +14126,8 @@
         <f>O5-I5</f>
         <v>0</v>
       </c>
-      <c r="R5" s="670"/>
-      <c r="S5" s="670"/>
+      <c r="R5" s="667"/>
+      <c r="S5" s="667"/>
       <c r="T5" s="12"/>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
@@ -11791,8 +14180,8 @@
         <f>O6-I6</f>
         <v>-2</v>
       </c>
-      <c r="R6" s="671"/>
-      <c r="S6" s="671"/>
+      <c r="R6" s="668"/>
+      <c r="S6" s="668"/>
       <c r="T6" s="180" t="s">
         <v>79</v>
       </c>
@@ -11897,8 +14286,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R8" s="672"/>
-      <c r="S8" s="672"/>
+      <c r="R8" s="669"/>
+      <c r="S8" s="669"/>
       <c r="T8" s="45"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
@@ -11985,8 +14374,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R10" s="673"/>
-      <c r="S10" s="673"/>
+      <c r="R10" s="670"/>
+      <c r="S10" s="670"/>
       <c r="T10" s="45"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -12137,8 +14526,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R13" s="674"/>
-      <c r="S13" s="674"/>
+      <c r="R13" s="671"/>
+      <c r="S13" s="671"/>
       <c r="T13" s="45"/>
       <c r="U13" s="66"/>
       <c r="V13" s="66"/>
@@ -12471,8 +14860,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R20" s="675"/>
-      <c r="S20" s="675"/>
+      <c r="R20" s="672"/>
+      <c r="S20" s="672"/>
       <c r="T20" s="45"/>
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
@@ -12559,8 +14948,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R22" s="676"/>
-      <c r="S22" s="676"/>
+      <c r="R22" s="673"/>
+      <c r="S22" s="673"/>
       <c r="T22" s="45"/>
       <c r="U22" s="78"/>
       <c r="V22" s="78"/>
@@ -12609,8 +14998,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R23" s="677"/>
-      <c r="S23" s="677"/>
+      <c r="R23" s="674"/>
+      <c r="S23" s="674"/>
       <c r="T23" s="180" t="s">
         <v>80</v>
       </c>
@@ -12749,8 +15138,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R26" s="678"/>
-      <c r="S26" s="678"/>
+      <c r="R26" s="675"/>
+      <c r="S26" s="675"/>
       <c r="T26" s="45"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
@@ -13854,10 +16243,10 @@
     <row r="51" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="695" t="s">
+      <c r="F51" s="704" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="695"/>
+      <c r="G51" s="704"/>
       <c r="H51" s="148">
         <f>SUM(H5:H34)</f>
         <v>74525.02</v>
@@ -14085,6 +16474,14 @@
     <sortCondition ref="B5:B50"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
@@ -14097,14 +16494,6 @@
     <mergeCell ref="R22:S22"/>
     <mergeCell ref="R23:S23"/>
     <mergeCell ref="R26:S26"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.31" bottom="0.3" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="90" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14147,10 +16536,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="653" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="654"/>
+      <c r="B1" s="676" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="677"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -14165,26 +16554,26 @@
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="2:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="679">
+      <c r="B2" s="688">
         <v>45056</v>
       </c>
-      <c r="C2" s="680"/>
-      <c r="F2" s="681" t="s">
+      <c r="C2" s="689"/>
+      <c r="F2" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="682"/>
-      <c r="H2" s="683"/>
-      <c r="I2" s="684"/>
-      <c r="J2" s="685" t="s">
+      <c r="G2" s="691"/>
+      <c r="H2" s="692"/>
+      <c r="I2" s="693"/>
+      <c r="J2" s="694" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="685"/>
-      <c r="L2" s="686"/>
+      <c r="K2" s="694"/>
+      <c r="L2" s="695"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="658" t="s">
+      <c r="N2" s="681" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="658"/>
+      <c r="O2" s="681"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
       <c r="T2" s="12"/>
@@ -14194,33 +16583,33 @@
     </row>
     <row r="3" spans="2:27" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="689" t="s">
+      <c r="C3" s="698" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="690"/>
+      <c r="D3" s="699"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="691" t="s">
+      <c r="F3" s="700" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="692"/>
+      <c r="G3" s="701"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="693" t="s">
+      <c r="I3" s="702" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="687"/>
-      <c r="K3" s="687"/>
-      <c r="L3" s="688"/>
+      <c r="J3" s="696"/>
+      <c r="K3" s="696"/>
+      <c r="L3" s="697"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="658"/>
-      <c r="O3" s="658"/>
-      <c r="P3" s="666" t="s">
+      <c r="N3" s="681"/>
+      <c r="O3" s="681"/>
+      <c r="P3" s="663" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="667"/>
-      <c r="R3" s="668" t="s">
+      <c r="Q3" s="664"/>
+      <c r="R3" s="665" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="669"/>
+      <c r="S3" s="666"/>
       <c r="T3" s="12"/>
       <c r="U3" s="13"/>
       <c r="V3" s="13"/>
@@ -14246,7 +16635,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="694"/>
+      <c r="I4" s="703"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -14317,8 +16706,8 @@
         <f>I5-L5</f>
         <v>0</v>
       </c>
-      <c r="R5" s="670"/>
-      <c r="S5" s="670"/>
+      <c r="R5" s="667"/>
+      <c r="S5" s="667"/>
       <c r="T5" s="12"/>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
@@ -14367,8 +16756,8 @@
         <f>I6-L6</f>
         <v>0</v>
       </c>
-      <c r="R6" s="671"/>
-      <c r="S6" s="671"/>
+      <c r="R6" s="668"/>
+      <c r="S6" s="668"/>
       <c r="T6" s="180"/>
       <c r="U6" s="13"/>
       <c r="V6" s="46"/>
@@ -14463,8 +16852,8 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="R8" s="672"/>
-      <c r="S8" s="672"/>
+      <c r="R8" s="669"/>
+      <c r="S8" s="669"/>
       <c r="T8" s="45"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
@@ -14539,8 +16928,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R10" s="673"/>
-      <c r="S10" s="673"/>
+      <c r="R10" s="670"/>
+      <c r="S10" s="670"/>
       <c r="T10" s="45"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -14661,8 +17050,8 @@
         <f t="shared" si="2"/>
         <v>-3</v>
       </c>
-      <c r="R13" s="674"/>
-      <c r="S13" s="674"/>
+      <c r="R13" s="671"/>
+      <c r="S13" s="671"/>
       <c r="T13" s="45"/>
       <c r="U13" s="66"/>
       <c r="V13" s="66"/>
@@ -14943,8 +17332,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R20" s="675"/>
-      <c r="S20" s="675"/>
+      <c r="R20" s="672"/>
+      <c r="S20" s="672"/>
       <c r="T20" s="45"/>
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
@@ -15019,8 +17408,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R22" s="676"/>
-      <c r="S22" s="676"/>
+      <c r="R22" s="673"/>
+      <c r="S22" s="673"/>
       <c r="T22" s="45"/>
       <c r="U22" s="78"/>
       <c r="V22" s="78"/>
@@ -15065,8 +17454,8 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-      <c r="R23" s="677"/>
-      <c r="S23" s="677"/>
+      <c r="R23" s="674"/>
+      <c r="S23" s="674"/>
       <c r="T23" s="180"/>
       <c r="U23" s="13"/>
       <c r="V23" s="13"/>
@@ -15195,8 +17584,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R26" s="678"/>
-      <c r="S26" s="678"/>
+      <c r="R26" s="675"/>
+      <c r="S26" s="675"/>
       <c r="T26" s="45"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
@@ -16202,10 +18591,10 @@
     <row r="51" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="695" t="s">
+      <c r="F51" s="704" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="695"/>
+      <c r="G51" s="704"/>
       <c r="H51" s="148">
         <f>SUM(H5:H34)</f>
         <v>51160.97</v>
@@ -16428,14 +18817,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
@@ -16448,6 +18829,14 @@
     <mergeCell ref="R22:S22"/>
     <mergeCell ref="R23:S23"/>
     <mergeCell ref="R26:S26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -16491,10 +18880,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="653" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="654"/>
+      <c r="B1" s="676" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="677"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -16509,26 +18898,26 @@
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="2:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="679">
+      <c r="B2" s="688">
         <v>45082</v>
       </c>
-      <c r="C2" s="680"/>
-      <c r="F2" s="681" t="s">
+      <c r="C2" s="689"/>
+      <c r="F2" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="682"/>
-      <c r="H2" s="683"/>
-      <c r="I2" s="684"/>
-      <c r="J2" s="685" t="s">
+      <c r="G2" s="691"/>
+      <c r="H2" s="692"/>
+      <c r="I2" s="693"/>
+      <c r="J2" s="694" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="685"/>
-      <c r="L2" s="686"/>
+      <c r="K2" s="694"/>
+      <c r="L2" s="695"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="658" t="s">
+      <c r="N2" s="681" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="658"/>
+      <c r="O2" s="681"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
       <c r="T2" s="12"/>
@@ -16538,33 +18927,33 @@
     </row>
     <row r="3" spans="2:27" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="689" t="s">
+      <c r="C3" s="698" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="690"/>
+      <c r="D3" s="699"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="691" t="s">
+      <c r="F3" s="700" t="s">
         <v>93</v>
       </c>
-      <c r="G3" s="692"/>
+      <c r="G3" s="701"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="693" t="s">
+      <c r="I3" s="702" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="687"/>
-      <c r="K3" s="687"/>
-      <c r="L3" s="688"/>
+      <c r="J3" s="696"/>
+      <c r="K3" s="696"/>
+      <c r="L3" s="697"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="658"/>
-      <c r="O3" s="658"/>
-      <c r="P3" s="666" t="s">
+      <c r="N3" s="681"/>
+      <c r="O3" s="681"/>
+      <c r="P3" s="663" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="667"/>
-      <c r="R3" s="668" t="s">
+      <c r="Q3" s="664"/>
+      <c r="R3" s="665" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="669"/>
+      <c r="S3" s="666"/>
       <c r="T3" s="12"/>
       <c r="U3" s="13"/>
       <c r="V3" s="13"/>
@@ -16590,7 +18979,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="694"/>
+      <c r="I4" s="703"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -16653,8 +19042,8 @@
         <f>I5-L5</f>
         <v>0</v>
       </c>
-      <c r="R5" s="670"/>
-      <c r="S5" s="670"/>
+      <c r="R5" s="667"/>
+      <c r="S5" s="667"/>
       <c r="T5" s="12"/>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
@@ -16703,8 +19092,8 @@
         <f>O6-L6</f>
         <v>0</v>
       </c>
-      <c r="R6" s="671"/>
-      <c r="S6" s="671"/>
+      <c r="R6" s="668"/>
+      <c r="S6" s="668"/>
       <c r="T6" s="180"/>
       <c r="U6" s="13"/>
       <c r="V6" s="46"/>
@@ -16795,8 +19184,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R8" s="672"/>
-      <c r="S8" s="672"/>
+      <c r="R8" s="669"/>
+      <c r="S8" s="669"/>
       <c r="T8" s="45"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
@@ -16871,8 +19260,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R10" s="673"/>
-      <c r="S10" s="673"/>
+      <c r="R10" s="670"/>
+      <c r="S10" s="670"/>
       <c r="T10" s="45"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -17019,8 +19408,8 @@
         <f>O13-I13</f>
         <v>0</v>
       </c>
-      <c r="R13" s="674"/>
-      <c r="S13" s="674"/>
+      <c r="R13" s="671"/>
+      <c r="S13" s="671"/>
       <c r="T13" s="45"/>
       <c r="U13" s="66"/>
       <c r="V13" s="66"/>
@@ -17339,8 +19728,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R20" s="675"/>
-      <c r="S20" s="675"/>
+      <c r="R20" s="672"/>
+      <c r="S20" s="672"/>
       <c r="T20" s="45"/>
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
@@ -17427,8 +19816,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R22" s="676"/>
-      <c r="S22" s="676"/>
+      <c r="R22" s="673"/>
+      <c r="S22" s="673"/>
       <c r="T22" s="45"/>
       <c r="U22" s="78"/>
       <c r="V22" s="78"/>
@@ -17477,8 +19866,8 @@
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="R23" s="677"/>
-      <c r="S23" s="677"/>
+      <c r="R23" s="674"/>
+      <c r="S23" s="674"/>
       <c r="T23" s="347" t="s">
         <v>99</v>
       </c>
@@ -17629,8 +20018,8 @@
         <f t="shared" si="5"/>
         <v>-1</v>
       </c>
-      <c r="R26" s="678"/>
-      <c r="S26" s="678"/>
+      <c r="R26" s="675"/>
+      <c r="S26" s="675"/>
       <c r="T26" s="347" t="s">
         <v>99</v>
       </c>
@@ -18707,10 +21096,10 @@
     <row r="51" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="695" t="s">
+      <c r="F51" s="704" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="695"/>
+      <c r="G51" s="704"/>
       <c r="H51" s="148">
         <f>SUM(H5:H34)</f>
         <v>55132.759999999995</v>
@@ -18938,6 +21327,14 @@
     <sortCondition ref="B27:B47"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
@@ -18950,14 +21347,6 @@
     <mergeCell ref="R22:S22"/>
     <mergeCell ref="R23:S23"/>
     <mergeCell ref="R26:S26"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.27559055118110237" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19003,10 +21392,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="653" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="654"/>
+      <c r="B1" s="676" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="677"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -19020,30 +21409,30 @@
       <c r="R1" s="13"/>
     </row>
     <row r="2" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="701">
+      <c r="B2" s="710">
         <v>45108</v>
       </c>
-      <c r="C2" s="702"/>
-      <c r="F2" s="681" t="s">
+      <c r="C2" s="711"/>
+      <c r="F2" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="682"/>
-      <c r="H2" s="683"/>
-      <c r="I2" s="684"/>
-      <c r="J2" s="685" t="s">
+      <c r="G2" s="691"/>
+      <c r="H2" s="692"/>
+      <c r="I2" s="693"/>
+      <c r="J2" s="694" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="685"/>
-      <c r="L2" s="686"/>
+      <c r="K2" s="694"/>
+      <c r="L2" s="695"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="658" t="s">
+      <c r="N2" s="681" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="658"/>
-      <c r="P2" s="696" t="s">
+      <c r="O2" s="681"/>
+      <c r="P2" s="705" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="697"/>
+      <c r="Q2" s="706"/>
       <c r="S2" s="12"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
@@ -19051,27 +21440,27 @@
     </row>
     <row r="3" spans="2:26" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="689" t="s">
+      <c r="C3" s="698" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="690"/>
+      <c r="D3" s="699"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="691" t="s">
+      <c r="F3" s="700" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="692"/>
+      <c r="G3" s="701"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="693" t="s">
+      <c r="I3" s="702" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="687"/>
-      <c r="K3" s="687"/>
-      <c r="L3" s="688"/>
+      <c r="J3" s="696"/>
+      <c r="K3" s="696"/>
+      <c r="L3" s="697"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="658"/>
-      <c r="O3" s="658"/>
-      <c r="P3" s="698"/>
-      <c r="Q3" s="699"/>
+      <c r="N3" s="681"/>
+      <c r="O3" s="681"/>
+      <c r="P3" s="707"/>
+      <c r="Q3" s="708"/>
       <c r="R3" s="434"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
@@ -19098,7 +21487,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="694"/>
+      <c r="I4" s="703"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -19623,7 +22012,7 @@
         <v>-16</v>
       </c>
       <c r="R15" s="411"/>
-      <c r="S15" s="700" t="s">
+      <c r="S15" s="709" t="s">
         <v>109</v>
       </c>
       <c r="T15" s="13"/>
@@ -19674,7 +22063,7 @@
         <v>6</v>
       </c>
       <c r="R16" s="412"/>
-      <c r="S16" s="700"/>
+      <c r="S16" s="709"/>
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
@@ -21149,10 +23538,10 @@
     <row r="51" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="695" t="s">
+      <c r="F51" s="704" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="695"/>
+      <c r="G51" s="704"/>
       <c r="H51" s="148">
         <f>SUM(H5:H34)</f>
         <v>34034.630000000005</v>
@@ -21422,10 +23811,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="653" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="654"/>
+      <c r="B1" s="676" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="677"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -21439,30 +23828,30 @@
       <c r="R1" s="13"/>
     </row>
     <row r="2" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="701">
+      <c r="B2" s="710">
         <v>45136</v>
       </c>
-      <c r="C2" s="702"/>
-      <c r="F2" s="681" t="s">
+      <c r="C2" s="711"/>
+      <c r="F2" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="682"/>
-      <c r="H2" s="683"/>
-      <c r="I2" s="684"/>
-      <c r="J2" s="685" t="s">
+      <c r="G2" s="691"/>
+      <c r="H2" s="692"/>
+      <c r="I2" s="693"/>
+      <c r="J2" s="694" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="685"/>
-      <c r="L2" s="686"/>
+      <c r="K2" s="694"/>
+      <c r="L2" s="695"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="703" t="s">
+      <c r="N2" s="712" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="703"/>
-      <c r="P2" s="696" t="s">
+      <c r="O2" s="712"/>
+      <c r="P2" s="705" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="697"/>
+      <c r="Q2" s="706"/>
       <c r="S2" s="12"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
@@ -21470,27 +23859,27 @@
     </row>
     <row r="3" spans="2:26" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="689" t="s">
+      <c r="C3" s="698" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="690"/>
+      <c r="D3" s="699"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="691" t="s">
+      <c r="F3" s="700" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="692"/>
+      <c r="G3" s="701"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="693" t="s">
+      <c r="I3" s="702" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="687"/>
-      <c r="K3" s="687"/>
-      <c r="L3" s="688"/>
+      <c r="J3" s="696"/>
+      <c r="K3" s="696"/>
+      <c r="L3" s="697"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="703"/>
-      <c r="O3" s="703"/>
-      <c r="P3" s="698"/>
-      <c r="Q3" s="699"/>
+      <c r="N3" s="712"/>
+      <c r="O3" s="712"/>
+      <c r="P3" s="707"/>
+      <c r="Q3" s="708"/>
       <c r="R3" s="434"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
@@ -21517,7 +23906,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="694"/>
+      <c r="I4" s="703"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -23472,10 +25861,10 @@
     <row r="51" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="695" t="s">
+      <c r="F51" s="704" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="695"/>
+      <c r="G51" s="704"/>
       <c r="H51" s="148">
         <f>SUM(H5:H34)</f>
         <v>42356.71</v>
@@ -23696,16 +26085,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L3"/>
     <mergeCell ref="N2:O3"/>
     <mergeCell ref="P2:Q3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L3"/>
   </mergeCells>
   <pageMargins left="0.39" right="0.23622047244094491" top="0.31496062992125984" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="65" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -23748,10 +26137,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="706" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="706"/>
+      <c r="B1" s="715" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="715"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -23769,26 +26158,26 @@
         <v>45171</v>
       </c>
       <c r="C2" s="570"/>
-      <c r="F2" s="681" t="s">
+      <c r="F2" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="682"/>
-      <c r="H2" s="683"/>
-      <c r="I2" s="684"/>
-      <c r="J2" s="685" t="s">
+      <c r="G2" s="691"/>
+      <c r="H2" s="692"/>
+      <c r="I2" s="693"/>
+      <c r="J2" s="694" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="685"/>
-      <c r="L2" s="686"/>
+      <c r="K2" s="694"/>
+      <c r="L2" s="695"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="703" t="s">
+      <c r="N2" s="712" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="703"/>
-      <c r="P2" s="696" t="s">
+      <c r="O2" s="712"/>
+      <c r="P2" s="705" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="697"/>
+      <c r="Q2" s="706"/>
       <c r="S2" s="12"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
@@ -23796,27 +26185,27 @@
     </row>
     <row r="3" spans="2:26" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="568"/>
-      <c r="C3" s="707" t="s">
+      <c r="C3" s="716" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="690"/>
+      <c r="D3" s="699"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="691" t="s">
+      <c r="F3" s="700" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="692"/>
+      <c r="G3" s="701"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="693" t="s">
+      <c r="I3" s="702" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="687"/>
-      <c r="K3" s="687"/>
-      <c r="L3" s="688"/>
+      <c r="J3" s="696"/>
+      <c r="K3" s="696"/>
+      <c r="L3" s="697"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="703"/>
-      <c r="O3" s="703"/>
-      <c r="P3" s="698"/>
-      <c r="Q3" s="699"/>
+      <c r="N3" s="712"/>
+      <c r="O3" s="712"/>
+      <c r="P3" s="707"/>
+      <c r="Q3" s="708"/>
       <c r="R3" s="434"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
@@ -23843,7 +26232,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="694"/>
+      <c r="I4" s="703"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -24327,10 +26716,10 @@
         <v>3</v>
       </c>
       <c r="M15" s="526"/>
-      <c r="N15" s="708">
+      <c r="N15" s="717">
         <v>96.813999999999993</v>
       </c>
-      <c r="O15" s="710">
+      <c r="O15" s="719">
         <v>3</v>
       </c>
       <c r="P15" s="562">
@@ -24342,7 +26731,7 @@
         <v>1</v>
       </c>
       <c r="R15" s="411"/>
-      <c r="S15" s="704" t="s">
+      <c r="S15" s="713" t="s">
         <v>137</v>
       </c>
       <c r="T15" s="13"/>
@@ -24374,8 +26763,8 @@
       <c r="K16" s="528"/>
       <c r="L16" s="529"/>
       <c r="M16" s="526"/>
-      <c r="N16" s="709"/>
-      <c r="O16" s="711"/>
+      <c r="N16" s="718"/>
+      <c r="O16" s="720"/>
       <c r="P16" s="562">
         <f t="shared" si="3"/>
         <v>-33.090000000000003</v>
@@ -24385,7 +26774,7 @@
         <v>0</v>
       </c>
       <c r="R16" s="412"/>
-      <c r="S16" s="705"/>
+      <c r="S16" s="714"/>
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
@@ -25806,10 +28195,10 @@
     <row r="51" spans="2:22" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="695" t="s">
+      <c r="F51" s="704" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="695"/>
+      <c r="G51" s="704"/>
       <c r="H51" s="560">
         <f>SUM(H5:H34)</f>
         <v>51673.75</v>
@@ -26086,10 +28475,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="706" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="706"/>
+      <c r="B1" s="715" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="715"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -26107,26 +28496,26 @@
         <v>45201</v>
       </c>
       <c r="C2" s="570"/>
-      <c r="F2" s="681" t="s">
+      <c r="F2" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="682"/>
-      <c r="H2" s="683"/>
-      <c r="I2" s="684"/>
-      <c r="J2" s="685" t="s">
+      <c r="G2" s="691"/>
+      <c r="H2" s="692"/>
+      <c r="I2" s="693"/>
+      <c r="J2" s="694" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="685"/>
-      <c r="L2" s="686"/>
+      <c r="K2" s="694"/>
+      <c r="L2" s="695"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="703" t="s">
+      <c r="N2" s="712" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="703"/>
-      <c r="P2" s="712" t="s">
+      <c r="O2" s="712"/>
+      <c r="P2" s="726" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="713"/>
+      <c r="Q2" s="727"/>
       <c r="S2" s="12"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
@@ -26134,27 +28523,27 @@
     </row>
     <row r="3" spans="2:26" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="568"/>
-      <c r="C3" s="707" t="s">
+      <c r="C3" s="716" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="690"/>
+      <c r="D3" s="699"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="691" t="s">
+      <c r="F3" s="700" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="692"/>
+      <c r="G3" s="701"/>
       <c r="H3" s="586"/>
-      <c r="I3" s="716" t="s">
+      <c r="I3" s="730" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="687"/>
-      <c r="K3" s="687"/>
-      <c r="L3" s="688"/>
+      <c r="J3" s="696"/>
+      <c r="K3" s="696"/>
+      <c r="L3" s="697"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="703"/>
-      <c r="O3" s="703"/>
-      <c r="P3" s="714"/>
-      <c r="Q3" s="715"/>
+      <c r="N3" s="712"/>
+      <c r="O3" s="712"/>
+      <c r="P3" s="728"/>
+      <c r="Q3" s="729"/>
       <c r="R3" s="434"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
@@ -26181,7 +28570,7 @@
       <c r="H4" s="587" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="717"/>
+      <c r="I4" s="731"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -26675,10 +29064,10 @@
         <v>103</v>
       </c>
       <c r="M15" s="526"/>
-      <c r="N15" s="718">
+      <c r="N15" s="721">
         <v>3617.26</v>
       </c>
-      <c r="O15" s="720">
+      <c r="O15" s="723">
         <v>141</v>
       </c>
       <c r="P15" s="597">
@@ -26690,7 +29079,7 @@
         <v>38</v>
       </c>
       <c r="R15" s="411"/>
-      <c r="S15" s="722" t="s">
+      <c r="S15" s="725" t="s">
         <v>145</v>
       </c>
       <c r="T15" s="13"/>
@@ -26718,8 +29107,8 @@
       <c r="K16" s="524"/>
       <c r="L16" s="525"/>
       <c r="M16" s="526"/>
-      <c r="N16" s="719"/>
-      <c r="O16" s="721"/>
+      <c r="N16" s="722"/>
+      <c r="O16" s="724"/>
       <c r="P16" s="597">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -26729,7 +29118,7 @@
         <v>0</v>
       </c>
       <c r="R16" s="412"/>
-      <c r="S16" s="722"/>
+      <c r="S16" s="725"/>
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
@@ -26934,7 +29323,7 @@
         <v>-35</v>
       </c>
       <c r="R21" s="413"/>
-      <c r="S21" s="722" t="s">
+      <c r="S21" s="725" t="s">
         <v>145</v>
       </c>
       <c r="T21" s="77"/>
@@ -26973,7 +29362,7 @@
         <v>0</v>
       </c>
       <c r="R22" s="577"/>
-      <c r="S22" s="722"/>
+      <c r="S22" s="725"/>
       <c r="T22" s="78"/>
       <c r="U22" s="78"/>
       <c r="V22" s="13"/>
@@ -27022,7 +29411,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="578"/>
-      <c r="S23" s="722" t="s">
+      <c r="S23" s="725" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="13"/>
@@ -27061,7 +29450,7 @@
         <v>0</v>
       </c>
       <c r="R24" s="414"/>
-      <c r="S24" s="722"/>
+      <c r="S24" s="725"/>
       <c r="T24" s="13"/>
       <c r="U24" s="13"/>
       <c r="V24" s="13"/>
@@ -28164,10 +30553,10 @@
     <row r="51" spans="2:22" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="695" t="s">
+      <c r="F51" s="704" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="695"/>
+      <c r="G51" s="704"/>
       <c r="H51" s="560">
         <f>SUM(H5:H34)</f>
         <v>22552.550000000003</v>
@@ -28371,12 +30760,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="S21:S22"/>
-    <mergeCell ref="S23:S24"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:L3"/>
@@ -28385,6 +30768,12 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:I4"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="S21:S22"/>
+    <mergeCell ref="S23:S24"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.23622047244094491" top="0.35433070866141736" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>